<commit_message>
Updated lapse spreadsheet and copied files from Ncristea
</commit_message>
<xml_diff>
--- a/Lape rate plots.xlsx
+++ b/Lape rate plots.xlsx
@@ -1,30 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbeaulieu\Desktop\Lapse Rate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cband\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF55D0C-4B69-40B1-AA8A-D0A4ABA437C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17400" windowHeight="6525"/>
+    <workbookView xWindow="675" yWindow="158" windowWidth="19530" windowHeight="12052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$15:$B$16</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$16:$B$17</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$15:$C$16</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$16:$C$17</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Elevation KM</t>
   </si>
@@ -32,23 +45,53 @@
     <t>T (daily mean)</t>
   </si>
   <si>
-    <t>Lapse 1</t>
+    <t>NRN1</t>
   </si>
   <si>
-    <t>Lapse 7</t>
+    <t>NRN7</t>
   </si>
   <si>
-    <t>Lapse 5</t>
+    <t>NRN5-7</t>
   </si>
   <si>
-    <t>make for May 2018</t>
+    <t>NRN1-5</t>
+  </si>
+  <si>
+    <t>NFN1-7</t>
+  </si>
+  <si>
+    <t>CONUS (-6.5)</t>
+  </si>
+  <si>
+    <t>N. Cascades (-4.5)</t>
+  </si>
+  <si>
+    <t>meters</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>NFN1-NFN3</t>
+  </si>
+  <si>
+    <t>NFN3-NFN4</t>
+  </si>
+  <si>
+    <t>NFN4-NFN5</t>
+  </si>
+  <si>
+    <t>NFN5-NFN7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +105,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -71,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,14 +128,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -106,7 +178,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -120,7 +192,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Curved Lapse Rate</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050"/>
+              <a:t>Daily</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t> Average Temperatures from 2018</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -159,6 +269,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NRN1-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -171,21 +292,24 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent6"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -195,7 +319,12 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.5489351527394154"/>
+                  <c:y val="5.085910070377795E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -228,7 +357,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$6</c:f>
+              <c:f>Sheet1!$B$15:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -236,14 +365,14 @@
                   <c:v>0.50687000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.74306614</c:v>
+                  <c:v>1.28649802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$6</c:f>
+              <c:f>Sheet1!$C$15:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -251,247 +380,32 @@
                   <c:v>8.0129335499999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.77108094</c:v>
+                  <c:v>4.2009345199999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-78E7-4095-BEC0-07F75439284C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="309650832"/>
-        <c:axId val="309649712"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="309650832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="309649712"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="309649712"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="309650832"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NRN5-7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -504,21 +418,24 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent5"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
@@ -530,8 +447,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.7309831222992534E-2"/>
-                  <c:y val="7.975690797183857E-2"/>
+                  <c:x val="0.44128622665622297"/>
+                  <c:y val="7.7840144893420046E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -595,112 +512,16 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$15:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.50687000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.28649802</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$15:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>8.0129335499999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2009345199999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-78E7-4095-BEC0-07F75439284C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -730,6 +551,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elevation (kilometers)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -792,6 +668,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  degrees (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -841,6 +777,1804 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.61755616935317648"/>
+          <c:y val="0.25390714846836698"/>
+          <c:w val="0.34753981668521799"/>
+          <c:h val="0.43294306476090161"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Linear Lapse Rates</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="900"/>
+              <a:t>NFN1 and NFN7 Daily</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="900" baseline="0"/>
+              <a:t> Average Temperatures from 2018</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21080265490373912"/>
+          <c:y val="2.9357792509756071E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFN1-7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.42349587880462308"/>
+                  <c:y val="4.182021395743428E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.50687000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.74306614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.0129335499999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.77108094</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B0B7-4A7A-8404-FFCF3D2A06C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CONUS (-6.5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.3834958788046231"/>
+                  <c:y val="-3.9910801625697392E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.50687000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.74306614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.8673450000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.1679299099999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B0B7-4A7A-8404-FFCF3D2A06C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N. Cascades (-4.5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.380571902196436"/>
+                  <c:y val="0.29421246951046842"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = -4.5x + 10.162</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" baseline="0"/>
+                    </a:br>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.50687000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.74306614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.8810850000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3182023700000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B0B7-4A7A-8404-FFCF3D2A06C4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="308022416"/>
+        <c:axId val="380162720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="308022416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elevation (kilometers)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="380162720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="380162720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  degrees (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="308022416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.61824077911313713"/>
+          <c:y val="0.18540563261226947"/>
+          <c:w val="0.34753981668521799"/>
+          <c:h val="0.74617953792683878"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>May Lapse Rates</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="900"/>
+              <a:t>NFN1 and NFN7 Daily</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="900" baseline="0"/>
+              <a:t> Average Temperatures from 2018</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21080265490373912"/>
+          <c:y val="2.9357792509756071E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFN1-NFN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.65709424977044117"/>
+                  <c:y val="0.30924622373859023"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$28:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.50687000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66988000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$28:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12.984738</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.083333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1411-43F0-A757-01AF77CAD174}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFN3-NFN4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.53147082551502889"/>
+                  <c:y val="0.32045418327734032"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$29:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.66988000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0601500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12.083333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.548387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1411-43F0-A757-01AF77CAD174}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFN4-NFN5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.48063383066663562"/>
+                  <c:y val="0.23506966033240506"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$30:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0601500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2738800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$30:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10.548387</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9140160000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1411-43F0-A757-01AF77CAD174}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFN5-NFN7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.32732456929961795"/>
+                  <c:y val="0.34052218471939932"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.2738800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7468900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$31:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.9140160000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1426170000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1411-43F0-A757-01AF77CAD174}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="308022416"/>
+        <c:axId val="380162720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="308022416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Elevation (kilometers)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="380162720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="380162720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  degrees (C)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="308022416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7402615500618811"/>
+          <c:y val="0.20414049886881966"/>
+          <c:w val="0.2457052368014089"/>
+          <c:h val="0.62348805860193413"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -879,13 +2613,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -958,6 +2689,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1990,24 +3761,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2027,19 +4320,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>461963</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>271463</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBBD4901-EAB4-46B5-A3ED-FEA05D05BC87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2051,6 +4350,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25858AD5-38AA-4538-B6FD-04A281AE268D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2321,30 +4658,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2354,8 +4697,16 @@
       <c r="C5" s="1">
         <v>8.0129335499999996</v>
       </c>
+      <c r="D5">
+        <f>-6.5*B5+10.162</f>
+        <v>6.8673450000000003</v>
+      </c>
+      <c r="E5">
+        <f>-4.5*B5+10.162</f>
+        <v>7.8810850000000006</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2365,21 +4716,29 @@
       <c r="C6">
         <v>2.77108094</v>
       </c>
+      <c r="D6">
+        <f>-6.5*B6+10.162</f>
+        <v>-1.1679299099999998</v>
+      </c>
+      <c r="E6">
+        <f>-4.5*B6+10.162</f>
+        <v>2.3182023700000007</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C12" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>0.50687000000000004</v>
@@ -2388,7 +4747,7 @@
         <v>8.0129335499999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2399,9 +4758,9 @@
         <v>4.2009345199999997</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>1.74306614</v>
@@ -2410,14 +4769,115 @@
         <v>2.77108094</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B26" s="3">
+        <v>43221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <f>D28/1000</f>
+        <v>0.50687000000000004</v>
+      </c>
+      <c r="C28">
+        <v>12.984738</v>
+      </c>
+      <c r="D28" s="5">
+        <v>506.87</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ref="B29:B32" si="0">D29/1000</f>
+        <v>0.66988000000000003</v>
+      </c>
+      <c r="C29">
+        <v>12.083333</v>
+      </c>
+      <c r="D29" s="5">
+        <v>669.88</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0601500000000001</v>
+      </c>
+      <c r="C30">
+        <v>10.548387</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1060.1500000000001</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
         <v>5</v>
       </c>
+      <c r="B31" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2738800000000001</v>
+      </c>
+      <c r="C31">
+        <v>6.9140160000000002</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1273.8800000000001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="2">
+        <v>7</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7468900000000001</v>
+      </c>
+      <c r="C32">
+        <v>7.1426170000000004</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1746.89</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>